<commit_message>
try to generate new updated excel but get failed
</commit_message>
<xml_diff>
--- a/name.xlsx
+++ b/name.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="9">
   <si>
     <t>Url</t>
   </si>
@@ -37,70 +37,7 @@
     <t xml:space="preserve"> Name 4</t>
   </si>
   <si>
-    <t xml:space="preserve"> Name 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 24</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name 26</t>
+    <t/>
   </si>
   <si>
     <t xml:space="preserve"> Name 27</t>
@@ -167,12 +104,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -486,8 +426,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="33.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="33.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -531,179 +471,179 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>12</v>
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>14</v>
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>16</v>
+      <c r="A15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>17</v>
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>18</v>
+      <c r="A17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>19</v>
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>20</v>
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>21</v>
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>22</v>
+      <c r="A21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>23</v>
+      <c r="A22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>24</v>
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>25</v>
+      <c r="A24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>26</v>
+      <c r="A25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>27</v>
+      <c r="A26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>28</v>
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
@@ -711,7 +651,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>